<commit_message>
console facrtura-pks7 to txt files done
</commit_message>
<xml_diff>
--- a/cabinet/web/docs/faktura_all_template.xlsx
+++ b/cabinet/web/docs/faktura_all_template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akhad\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D021301-BD5B-4BD6-A9B7-1E3B23EBEA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="шаблон сч.фактура" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>onlinefactura.uz</t>
   </si>
@@ -261,13 +267,16 @@
   </si>
   <si>
     <t>Етказиб бериш киймати / Стоимость поставки</t>
+  </si>
+  <si>
+    <t>каталог коди</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -382,12 +391,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -420,6 +455,18 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -441,25 +488,27 @@
     <xf numFmtId="4" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="distributed" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный_Экспорт счет-фактура" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный_Экспорт счет-фактура" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -480,7 +529,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 3"/>
+        <xdr:cNvPr id="2" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -515,9 +570,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -555,9 +610,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -589,9 +644,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,9 +696,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -798,163 +889,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" customWidth="1"/>
+    <col min="2" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="39">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.6">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1">
-      <c r="B2" s="17" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1">
-      <c r="B3" s="17" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A4" s="18" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
+      <c r="B5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" s="10" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" s="10" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="E7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="F7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="G7" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="14"/>
+      <c r="I7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="J7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="14"/>
+      <c r="L7" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="10" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="13" t="s">
+    <row r="8" spans="1:12" s="10" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="14"/>
+      <c r="J8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -988,8 +1089,11 @@
       <c r="K9" s="8">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -997,54 +1101,58 @@
         <v>67</v>
       </c>
       <c r="C10">
+        <v>4911</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>1000</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>20</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>200</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1200</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>15</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>180</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>1380</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange password="CCF9" sqref="F1:IT9 A1:E8 A9:K9" name="Диапазон1"/>
+    <protectedRange password="CCF9" sqref="G1:IU9 A1:F8 A9:L9" name="Диапазон1"/>
   </protectedRanges>
-  <mergeCells count="16">
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:K8"/>
+  <mergeCells count="17">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:K3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:J3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1052,16 +1160,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -1072,7 +1180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1080,7 +1188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1088,7 +1196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1096,7 +1204,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1104,7 +1212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1112,7 +1220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1120,7 +1228,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1128,7 +1236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1136,7 +1244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1144,7 +1252,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1152,7 +1260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1160,7 +1268,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1168,7 +1276,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1176,7 +1284,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1184,7 +1292,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1192,7 +1300,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1200,7 +1308,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1208,7 +1316,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1216,7 +1324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1224,7 +1332,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1232,7 +1340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1240,7 +1348,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1248,7 +1356,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1256,7 +1364,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1264,7 +1372,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1272,7 +1380,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1280,7 +1388,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1288,7 +1396,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1296,7 +1404,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1304,7 +1412,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1312,7 +1420,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1320,7 +1428,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1328,7 +1436,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1336,7 +1444,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1344,7 +1452,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1352,7 +1460,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1360,7 +1468,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1368,7 +1476,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1376,7 +1484,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1384,7 +1492,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1392,7 +1500,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1400,7 +1508,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1408,7 +1516,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1416,7 +1524,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1424,7 +1532,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1432,7 +1540,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1440,7 +1548,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1448,7 +1556,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1456,7 +1564,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1464,7 +1572,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1472,7 +1580,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1480,7 +1588,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1488,7 +1596,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1496,7 +1604,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1504,7 +1612,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1512,7 +1620,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1520,7 +1628,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1528,7 +1636,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1536,7 +1644,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>

</xml_diff>